<commit_message>
Updated SeleniumDemo file with maven framework
</commit_message>
<xml_diff>
--- a/TestData/TDR.xlsx
+++ b/TestData/TDR.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLogin" sheetId="4" r:id="rId2"/>
     <sheet name="BlankLogin" sheetId="5" r:id="rId3"/>
     <sheet name="AddCustomer" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="OrangeHRM" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t xml:space="preserve"> vmdnbdn</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Admin2</t>
+  </si>
+  <si>
+    <t>Admin3</t>
   </si>
 </sst>
 </file>
@@ -534,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -596,12 +605,51 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>